<commit_message>
add license to cci collections
</commit_message>
<xml_diff>
--- a/data/cci/cci-collections.xlsx
+++ b/data/cci/cci-collections.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies/data/cci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FBE7A58-F922-D34F-AFAE-D65F5F3B7FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0771CEDE-38D4-E44C-8C23-8428639ADC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{582DAA99-A787-7B46-8AC4-4B4B2F4DDD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>URI</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>The sensors that have been used in the collection of the data for the ESA Climate Change Initiative (CCI).</t>
+  </si>
+  <si>
+    <t>Rights</t>
+  </si>
+  <si>
+    <t>This work is licensed under a BSD license.</t>
   </si>
 </sst>
 </file>
@@ -283,7 +289,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -297,17 +303,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -648,21 +648,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E7AEDF-F189-874B-B648-68CB3AE7EA90}">
-  <dimension ref="A1:XFD11"/>
+  <dimension ref="A1:AMA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="31" style="7" customWidth="1"/>
-    <col min="2" max="3" width="31.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="107.5" style="7" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="7" customWidth="1"/>
-    <col min="9" max="1014" width="10.6640625" style="7" customWidth="1"/>
-    <col min="1015" max="1015" width="13.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="31" style="6" customWidth="1"/>
+    <col min="2" max="3" width="31.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="107.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" style="6" customWidth="1"/>
+    <col min="10" max="1014" width="10.6640625" style="6" customWidth="1"/>
+    <col min="1015" max="1015" width="13.33203125" style="6" customWidth="1"/>
     <col min="1016" max="1024" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -691,7 +694,9 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -1703,19 +1708,19 @@
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1724,22 +1729,25 @@
       <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="I2" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:1015" ht="28">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1747,23 +1755,26 @@
       </c>
       <c r="H3" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:1015" ht="28">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1771,25 +1782,28 @@
       </c>
       <c r="H4" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1015" ht="28">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1797,6 +1811,9 @@
       </c>
       <c r="H5" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1015" ht="28">
@@ -1806,14 +1823,14 @@
       <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1821,6 +1838,9 @@
       </c>
       <c r="H6" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:1015" ht="28">
@@ -1830,14 +1850,14 @@
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -1845,6 +1865,9 @@
       </c>
       <c r="H7" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1015" ht="28">
@@ -1854,14 +1877,14 @@
       <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>40</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -1869,6 +1892,9 @@
       </c>
       <c r="H8" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:1015" ht="28">
@@ -1878,14 +1904,14 @@
       <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>44</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1893,6 +1919,9 @@
       </c>
       <c r="H9" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:1015" ht="28">
@@ -1902,14 +1931,14 @@
       <c r="B10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -1917,6 +1946,9 @@
       </c>
       <c r="H10" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:1015" ht="28">
@@ -1926,14 +1958,14 @@
       <c r="B11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>52</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -1941,6 +1973,9 @@
       </c>
       <c r="H11" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add "project" to the xlsx files
</commit_message>
<xml_diff>
--- a/data/cci/cci-collections.xlsx
+++ b/data/cci/cci-collections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies/data/cci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0771CEDE-38D4-E44C-8C23-8428639ADC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CBEDFA-3563-8948-8E69-E8BC462C8F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{582DAA99-A787-7B46-8AC4-4B4B2F4DDD25}"/>
+    <workbookView xWindow="-70280" yWindow="-1500" windowWidth="30240" windowHeight="18880" xr2:uid="{582DAA99-A787-7B46-8AC4-4B4B2F4DDD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
     <t>URI</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>This work is licensed under a BSD license.</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>This collection represents the projects within the CCI project</t>
+  </si>
+  <si>
+    <t>The different projects within the ESA Climate Change Initiative (CCI).</t>
   </si>
 </sst>
 </file>
@@ -648,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E7AEDF-F189-874B-B648-68CB3AE7EA90}">
-  <dimension ref="A1:AMA11"/>
+  <dimension ref="A1:AMA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -1953,20 +1965,20 @@
     </row>
     <row r="11" spans="1:1015" ht="28">
       <c r="A11" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>14</v>
@@ -1975,6 +1987,33 @@
         <v>15</v>
       </c>
       <c r="I11" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1015" ht="28">
+      <c r="A12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>